<commit_message>
most recent excel files
</commit_message>
<xml_diff>
--- a/APMLA/Test.xlsx
+++ b/APMLA/Test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="224">
   <si>
     <t>Equipment Number</t>
   </si>
@@ -281,18 +281,6 @@
     <t>SEGU5143467</t>
   </si>
   <si>
-    <t>MSKU3777094</t>
-  </si>
-  <si>
-    <t>DJLAXA3838786</t>
-  </si>
-  <si>
-    <t>7075358801</t>
-  </si>
-  <si>
-    <t>580834303</t>
-  </si>
-  <si>
     <t>SEGU6008369</t>
   </si>
   <si>
@@ -374,36 +362,6 @@
     <t>QSWB8174078</t>
   </si>
   <si>
-    <t>CAIU4440709</t>
-  </si>
-  <si>
-    <t>HYUNDAI FAITH</t>
-  </si>
-  <si>
-    <t>079E</t>
-  </si>
-  <si>
-    <t>7075360469</t>
-  </si>
-  <si>
-    <t>HDMUKGCA4872838</t>
-  </si>
-  <si>
-    <t>CAIU7488183</t>
-  </si>
-  <si>
-    <t>CAIU9976968</t>
-  </si>
-  <si>
-    <t>FSCU9630308</t>
-  </si>
-  <si>
-    <t>GAOU6213961</t>
-  </si>
-  <si>
-    <t>HDMU6863844</t>
-  </si>
-  <si>
     <t>BMOU4707781</t>
   </si>
   <si>
@@ -416,21 +374,12 @@
     <t>GJWB8464379</t>
   </si>
   <si>
-    <t>BMOU5087031</t>
+    <t>SEGU4674978</t>
   </si>
   <si>
     <t>065</t>
   </si>
   <si>
-    <t>7075366557</t>
-  </si>
-  <si>
-    <t>BUWB9298423</t>
-  </si>
-  <si>
-    <t>SEGU4674978</t>
-  </si>
-  <si>
     <t>7075358865</t>
   </si>
   <si>
@@ -452,138 +401,6 @@
     <t>HKWB8464904</t>
   </si>
   <si>
-    <t>BSIU9234218</t>
-  </si>
-  <si>
-    <t>7075360468</t>
-  </si>
-  <si>
-    <t>HDMUKGCA4872837</t>
-  </si>
-  <si>
-    <t>CAIU4353287</t>
-  </si>
-  <si>
-    <t>DFSU6389790</t>
-  </si>
-  <si>
-    <t>HDMU6883434</t>
-  </si>
-  <si>
-    <t>HMMU6158056</t>
-  </si>
-  <si>
-    <t>HMMU6192873</t>
-  </si>
-  <si>
-    <t>HMMU6286036</t>
-  </si>
-  <si>
-    <t>TCNU7703361</t>
-  </si>
-  <si>
-    <t>BSIU9205077</t>
-  </si>
-  <si>
-    <t>7075360466</t>
-  </si>
-  <si>
-    <t>HDMUKGCA4872807</t>
-  </si>
-  <si>
-    <t>CAIU7408721</t>
-  </si>
-  <si>
-    <t>CAXU9136711</t>
-  </si>
-  <si>
-    <t>DFSU6877182</t>
-  </si>
-  <si>
-    <t>DFSU6940449</t>
-  </si>
-  <si>
-    <t>DRYU9978391</t>
-  </si>
-  <si>
-    <t>HDMU6551907</t>
-  </si>
-  <si>
-    <t>HDMU6742122</t>
-  </si>
-  <si>
-    <t>HDMU6844253</t>
-  </si>
-  <si>
-    <t>HMMU6104358</t>
-  </si>
-  <si>
-    <t>HMMU6192493</t>
-  </si>
-  <si>
-    <t>HMMU6230818</t>
-  </si>
-  <si>
-    <t>TCLU8055651</t>
-  </si>
-  <si>
-    <t>TCLU8397510</t>
-  </si>
-  <si>
-    <t>TGBU6338011</t>
-  </si>
-  <si>
-    <t>BMOU5255285</t>
-  </si>
-  <si>
-    <t>7075360467</t>
-  </si>
-  <si>
-    <t>HDMUKGCA4872833</t>
-  </si>
-  <si>
-    <t>CAIU7200110</t>
-  </si>
-  <si>
-    <t>CAIU8159881</t>
-  </si>
-  <si>
-    <t>CAXU8161448</t>
-  </si>
-  <si>
-    <t>GESU6917959</t>
-  </si>
-  <si>
-    <t>HDMU6499579</t>
-  </si>
-  <si>
-    <t>HMMU6298783</t>
-  </si>
-  <si>
-    <t>TCLU5594053</t>
-  </si>
-  <si>
-    <t>TCNU5064636</t>
-  </si>
-  <si>
-    <t>TCNU7316526</t>
-  </si>
-  <si>
-    <t>TCNU7903837</t>
-  </si>
-  <si>
-    <t>TEMU7416762</t>
-  </si>
-  <si>
-    <t>TGBU5888862</t>
-  </si>
-  <si>
-    <t>TGBU6472329</t>
-  </si>
-  <si>
-    <t>TLLU5852238</t>
-  </si>
-  <si>
     <t>HDMU6575771</t>
   </si>
   <si>
@@ -602,18 +419,6 @@
     <t>HKWB8460786</t>
   </si>
   <si>
-    <t>TCNU1699963</t>
-  </si>
-  <si>
-    <t>DJLAXA3852239</t>
-  </si>
-  <si>
-    <t>7075361033</t>
-  </si>
-  <si>
-    <t>HDMUQSWB8098904</t>
-  </si>
-  <si>
     <t>7075364098</t>
   </si>
   <si>
@@ -659,6 +464,21 @@
     <t>HDMU6640901</t>
   </si>
   <si>
+    <t>MAGU2360361</t>
+  </si>
+  <si>
+    <t>EVER LIBRA</t>
+  </si>
+  <si>
+    <t>042E</t>
+  </si>
+  <si>
+    <t>7075368444</t>
+  </si>
+  <si>
+    <t>142900238803</t>
+  </si>
+  <si>
     <t>TCNU5749091</t>
   </si>
   <si>
@@ -668,6 +488,108 @@
     <t>NSNS493287</t>
   </si>
   <si>
+    <t>TCNU8653650</t>
+  </si>
+  <si>
+    <t>00066</t>
+  </si>
+  <si>
+    <t>DJLAXA3864528</t>
+  </si>
+  <si>
+    <t>7075375759</t>
+  </si>
+  <si>
+    <t>QSWB8174608</t>
+  </si>
+  <si>
+    <t>FSCU8501543</t>
+  </si>
+  <si>
+    <t>00071</t>
+  </si>
+  <si>
+    <t>7075364251</t>
+  </si>
+  <si>
+    <t>ZHWB1334433</t>
+  </si>
+  <si>
+    <t>GAOU6201364</t>
+  </si>
+  <si>
+    <t>CAXU8049588</t>
+  </si>
+  <si>
+    <t>7075368470</t>
+  </si>
+  <si>
+    <t>HDMUKGWB4875059</t>
+  </si>
+  <si>
+    <t>TEMU6937719</t>
+  </si>
+  <si>
+    <t>WFHU5202195</t>
+  </si>
+  <si>
+    <t>CAIU8438762</t>
+  </si>
+  <si>
+    <t>TCNU8208742</t>
+  </si>
+  <si>
+    <t>DRYU9160785</t>
+  </si>
+  <si>
+    <t>CAIU7200595</t>
+  </si>
+  <si>
+    <t>HDMU6667883</t>
+  </si>
+  <si>
+    <t>DFSU6225311</t>
+  </si>
+  <si>
+    <t>HDMU6887595</t>
+  </si>
+  <si>
+    <t>SEGU6003177</t>
+  </si>
+  <si>
+    <t>7075369315</t>
+  </si>
+  <si>
+    <t>QSWB8174252</t>
+  </si>
+  <si>
+    <t>HDMU6783498</t>
+  </si>
+  <si>
+    <t>MSKU7693480</t>
+  </si>
+  <si>
+    <t>SEALAND PHILADELPHIA</t>
+  </si>
+  <si>
+    <t>7075312968</t>
+  </si>
+  <si>
+    <t>580230949</t>
+  </si>
+  <si>
+    <t>HDMU4636625</t>
+  </si>
+  <si>
+    <t>DJLAXA3864552</t>
+  </si>
+  <si>
+    <t>7075367749</t>
+  </si>
+  <si>
+    <t>QSWB8174293</t>
+  </si>
+  <si>
     <t>CAIU6230717</t>
   </si>
   <si>
@@ -680,6 +602,42 @@
     <t>HDMUHKWB1863947</t>
   </si>
   <si>
+    <t>HDMU6517651</t>
+  </si>
+  <si>
+    <t>7075368471</t>
+  </si>
+  <si>
+    <t>HDMUKGWB4875064</t>
+  </si>
+  <si>
+    <t>CAIU7299657</t>
+  </si>
+  <si>
+    <t>TCNU9336820</t>
+  </si>
+  <si>
+    <t>CAIU7437144</t>
+  </si>
+  <si>
+    <t>TCLU8315960</t>
+  </si>
+  <si>
+    <t>CAIU9983735</t>
+  </si>
+  <si>
+    <t>HDMU6311125</t>
+  </si>
+  <si>
+    <t>TCNU4033604</t>
+  </si>
+  <si>
+    <t>TCLU5302423</t>
+  </si>
+  <si>
+    <t>HDMU6508032</t>
+  </si>
+  <si>
     <t>TCNU8518774</t>
   </si>
   <si>
@@ -690,6 +648,42 @@
   </si>
   <si>
     <t>HASU1335392</t>
+  </si>
+  <si>
+    <t>BMOU4590400</t>
+  </si>
+  <si>
+    <t>7075368472</t>
+  </si>
+  <si>
+    <t>HDMUKGWB4875070</t>
+  </si>
+  <si>
+    <t>TLLU5779862</t>
+  </si>
+  <si>
+    <t>TCLU7215668</t>
+  </si>
+  <si>
+    <t>TCNU8601132</t>
+  </si>
+  <si>
+    <t>CCLU6843540</t>
+  </si>
+  <si>
+    <t>TCNU7039993</t>
+  </si>
+  <si>
+    <t>TCLU6734191</t>
+  </si>
+  <si>
+    <t>HDMU6782552</t>
+  </si>
+  <si>
+    <t>7075375890</t>
+  </si>
+  <si>
+    <t>BUWB9299212</t>
   </si>
 </sst>
 </file>
@@ -734,7 +728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1205,44 +1199,44 @@
         <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>90</v>
       </c>
       <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" t="s">
         <v>94</v>
-      </c>
-      <c r="E25" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
         <v>66</v>
@@ -1251,24 +1245,24 @@
         <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
         <v>97</v>
@@ -1282,16 +1276,16 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
         <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" t="s">
-        <v>101</v>
       </c>
       <c r="E28" t="s">
         <v>101</v>
@@ -1314,15 +1308,15 @@
         <v>104</v>
       </c>
       <c r="E29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
         <v>105</v>
-      </c>
-      <c r="F29" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
@@ -1331,44 +1325,44 @@
         <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" t="s">
         <v>110</v>
       </c>
-      <c r="B31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" t="s">
-        <v>108</v>
-      </c>
       <c r="F31" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
         <v>113</v>
@@ -1385,13 +1379,13 @@
         <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
         <v>118</v>
@@ -1405,230 +1399,230 @@
         <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
         <v>122</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" t="s">
         <v>123</v>
-      </c>
-      <c r="E34" t="s">
-        <v>123</v>
-      </c>
-      <c r="F34" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
         <v>122</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" t="s">
         <v>123</v>
-      </c>
-      <c r="E35" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
         <v>122</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" t="s">
         <v>123</v>
-      </c>
-      <c r="E36" t="s">
-        <v>123</v>
-      </c>
-      <c r="F36" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
         <v>127</v>
       </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" t="s">
-        <v>123</v>
-      </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F37" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E39" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F39" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F43" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F44" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
         <v>144</v>
@@ -1637,1087 +1631,867 @@
         <v>144</v>
       </c>
       <c r="F45" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" t="s">
         <v>146</v>
       </c>
-      <c r="B46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>146</v>
+      </c>
+      <c r="F46" t="s">
         <v>147</v>
-      </c>
-      <c r="E46" t="s">
-        <v>147</v>
-      </c>
-      <c r="F46" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="s">
+        <v>146</v>
+      </c>
+      <c r="F47" t="s">
         <v>147</v>
-      </c>
-      <c r="E47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" t="s">
         <v>147</v>
-      </c>
-      <c r="E48" t="s">
-        <v>147</v>
-      </c>
-      <c r="F48" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" t="s">
         <v>151</v>
       </c>
-      <c r="B49" t="s">
-        <v>121</v>
-      </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="D51" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="E51" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F51" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="F52" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="D53" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="E53" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="F53" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F54" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F55" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E56" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F56" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F57" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F58" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F59" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E60" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F60" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E61" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F61" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E62" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F62" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E63" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F63" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="E64" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="F64" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="D65" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="E65" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="F65" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D66" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="E66" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="F66" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C67" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="D67" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="E67" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="F67" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B68" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="D68" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="E68" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="F68" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D69" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E69" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F69" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D70" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E70" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F70" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D71" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E71" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F71" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="B72" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F72" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D73" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E73" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F73" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D74" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E74" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F74" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D75" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E75" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F75" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E76" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F76" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="B77" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D77" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E77" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F77" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="B78" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D78" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="E78" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="F78" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D79" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="E79" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="F79" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="D80" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="E80" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
       <c r="F80" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D81" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="E81" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="F81" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D82" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="E82" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="F82" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="B83" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D83" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="E83" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="F83" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C84" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="D84" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="E84" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="D85" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="E85" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="F85" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
       </c>
       <c r="C86" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D86" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="E86" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="F86" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="D87" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="E87" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="F87" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D88" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E88" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="F88" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>204</v>
-      </c>
-      <c r="B89" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>82</v>
-      </c>
-      <c r="D89" t="s">
-        <v>205</v>
-      </c>
-      <c r="E89" t="s">
-        <v>205</v>
-      </c>
-      <c r="F89" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>193</v>
-      </c>
-      <c r="B90" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s">
-        <v>82</v>
-      </c>
-      <c r="D90" t="s">
-        <v>207</v>
-      </c>
-      <c r="E90" t="s">
-        <v>207</v>
-      </c>
-      <c r="F90" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>193</v>
-      </c>
-      <c r="B91" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s">
-        <v>82</v>
-      </c>
-      <c r="D91" t="s">
-        <v>208</v>
-      </c>
-      <c r="E91" t="s">
-        <v>208</v>
-      </c>
-      <c r="F91" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>193</v>
-      </c>
-      <c r="B92" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s">
-        <v>82</v>
-      </c>
-      <c r="D92" t="s">
-        <v>209</v>
-      </c>
-      <c r="E92" t="s">
-        <v>209</v>
-      </c>
-      <c r="F92" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>210</v>
-      </c>
-      <c r="B93" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s">
-        <v>82</v>
-      </c>
-      <c r="D93" t="s">
-        <v>211</v>
-      </c>
-      <c r="E93" t="s">
-        <v>211</v>
-      </c>
-      <c r="F93" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>213</v>
-      </c>
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>82</v>
-      </c>
-      <c r="D94" t="s">
-        <v>211</v>
-      </c>
-      <c r="E94" t="s">
-        <v>211</v>
-      </c>
-      <c r="F94" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>214</v>
-      </c>
-      <c r="B95" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" t="s">
-        <v>82</v>
-      </c>
-      <c r="D95" t="s">
-        <v>211</v>
-      </c>
-      <c r="E95" t="s">
-        <v>211</v>
-      </c>
-      <c r="F95" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>215</v>
-      </c>
-      <c r="B96" t="s">
-        <v>66</v>
-      </c>
-      <c r="C96" t="s">
-        <v>135</v>
-      </c>
-      <c r="D96" t="s">
-        <v>216</v>
-      </c>
-      <c r="E96" t="s">
-        <v>216</v>
-      </c>
-      <c r="F96" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>218</v>
-      </c>
-      <c r="B97" t="s">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s">
-        <v>219</v>
-      </c>
-      <c r="D97" t="s">
-        <v>220</v>
-      </c>
-      <c r="E97" t="s">
-        <v>220</v>
-      </c>
-      <c r="F97" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>222</v>
-      </c>
-      <c r="B98" t="s">
-        <v>7</v>
-      </c>
-      <c r="C98" t="s">
-        <v>82</v>
-      </c>
-      <c r="D98" t="s">
         <v>223</v>
-      </c>
-      <c r="E98" t="s">
-        <v>223</v>
-      </c>
-      <c r="F98" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>225</v>
-      </c>
-      <c r="B99" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" t="s">
-        <v>82</v>
-      </c>
-      <c r="D99" t="s">
-        <v>223</v>
-      </c>
-      <c r="E99" t="s">
-        <v>223</v>
-      </c>
-      <c r="F99" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>